<commit_message>
Updated the Sprint File
Update the week process
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint 11/Team05 Stand-up Meeting Sprint11.xlsx
+++ b/Project_Files/Sprint 11/Team05 Stand-up Meeting Sprint11.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\Sprint 11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547076\Desktop\FreebiesforNewbies\Project_Files\Sprint 11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32513B55-28FC-4463-8080-2FFB3317F08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17DD490-F322-409E-AD14-1B1F294D9D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1020" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Daily Stand-up Meeting Report</t>
   </si>
@@ -165,6 +165,24 @@
   </si>
   <si>
     <t>3) NA</t>
+  </si>
+  <si>
+    <t>Done the Queries for Events table</t>
+  </si>
+  <si>
+    <t>We are doing the next step of the project</t>
+  </si>
+  <si>
+    <t>We are preparing for the project presentation on databse</t>
+  </si>
+  <si>
+    <t>We have to do slides for Mid Term presentation</t>
+  </si>
+  <si>
+    <t>Done the prsentation slides and project details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present the presentation on midterm </t>
   </si>
 </sst>
 </file>
@@ -807,7 +825,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1411,9 +1429,15 @@
       <c r="A20" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1439,9 +1463,15 @@
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1467,9 +1497,15 @@
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>

</xml_diff>